<commit_message>
scraping 23-26 meet end
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TARIEL\Desktop\wrestling_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E9D20A-ED80-46AC-B4C8-B7A424F26B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CE7FC1-87C6-455A-9A8A-7D2F5C15EA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,7 +2464,7 @@
       <c r="E55" t="s">
         <v>25</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>158</v>
       </c>
       <c r="G55">
@@ -2510,7 +2510,7 @@
       <c r="E57" t="s">
         <v>25</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>162</v>
       </c>
       <c r="G57">
@@ -3891,6 +3891,8 @@
     <hyperlink ref="F116" r:id="rId13" xr:uid="{7A29123E-4890-4BC8-8E20-194D42252243}"/>
     <hyperlink ref="F61" r:id="rId14" xr:uid="{7B062950-F361-4611-9AB9-F4F8D590148A}"/>
     <hyperlink ref="F56" r:id="rId15" xr:uid="{3F37A577-3985-4239-A4C1-86024AE46A51}"/>
+    <hyperlink ref="F55" r:id="rId16" xr:uid="{19F70462-35D8-4BB0-9F69-FB49124B0447}"/>
+    <hyperlink ref="F57" r:id="rId17" xr:uid="{4042D759-F035-46E4-BB65-DB5F38BAC02A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
scraping video link login 10000-12900
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TARIEL\Desktop\wrestling_scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwin\data science academy\wrestling_scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CE7FC1-87C6-455A-9A8A-7D2F5C15EA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="344">
   <si>
     <t>tournament_name</t>
   </si>
@@ -821,12 +820,243 @@
   </si>
   <si>
     <t>https://uww.org/event/southeast-asian-wrestling-championships/results</t>
+  </si>
+  <si>
+    <t>Zagreb Open</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/zagreb-open-0/results</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>Ibrahim Moustafa</t>
+  </si>
+  <si>
+    <t>Alexandria, Egypt</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/ibrahim-moustafa-7/results</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-55/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-34/results</t>
+  </si>
+  <si>
+    <t>Astana, Kazakhstan</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/asian-championships-23/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-35/results</t>
+  </si>
+  <si>
+    <t>World Combat Games Qualifier</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-combat-games-qualifier/results</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-87/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/pan-american-championships-17/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/african-championships-6/results</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/african-championships-9/results</t>
+  </si>
+  <si>
+    <t>Kaba Uulu Kozhomkul &amp; Raatbek Sanatbaev</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/kaba-uulu-kozhomkul-raatbek-sanatbaev/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/asian-championships-24/results</t>
+  </si>
+  <si>
+    <t>Tirana, Albania</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-36/results</t>
+  </si>
+  <si>
+    <t>Seniors, U20, U17, U15, Veterans</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/asian-championships-33/results</t>
+  </si>
+  <si>
+    <t>Mexico City, Mexico</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/pan-american-championships-16/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/pan-american-championships-32/results</t>
+  </si>
+  <si>
+    <t>Santiago De Compostela, Spain</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-37/results</t>
+  </si>
+  <si>
+    <t>2nd African Beach Games</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/2nd-african-beach-games/results</t>
+  </si>
+  <si>
+    <t>Saint-Laurent-Du-Var, France</t>
+  </si>
+  <si>
+    <t>U20, U17</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-56/results</t>
+  </si>
+  <si>
+    <t>Saint-Laurent-Du-Var Beach Wrestling World Series</t>
+  </si>
+  <si>
+    <t>Beach Wrestling World Series</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/saint-laurent-du-var-beach-wrestling-world-series-1/results</t>
+  </si>
+  <si>
+    <t>Santiago, Chile</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/pan-american-championships-22/results</t>
+  </si>
+  <si>
+    <t>Kaposvar, Hungary</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/european-championships-48/results</t>
+  </si>
+  <si>
+    <t>Amman City, Jordan</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/asian-championships-25/results</t>
+  </si>
+  <si>
+    <t>Polyák Imre &amp; Varga János Memorial</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/polyak-imre-varga-janos-memorial/results</t>
+  </si>
+  <si>
+    <t>Jeux De La Francophonie</t>
+  </si>
+  <si>
+    <t>Kinshasa, Congo</t>
+  </si>
+  <si>
+    <t>FS, WW, AF</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/jeux-de-la-francophonie/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-53/results</t>
+  </si>
+  <si>
+    <t>Canberra, Australia</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/oceania-championships-3/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-65/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-85/results</t>
+  </si>
+  <si>
+    <t>11th Indian Ocean Islands Games</t>
+  </si>
+  <si>
+    <t>Antananarivo, Madagascar</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/11th-indian-ocean-islands-games/results</t>
+  </si>
+  <si>
+    <t>Constanta, Romania</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-50/results</t>
+  </si>
+  <si>
+    <t>3rd Mediterranean Beach Games</t>
+  </si>
+  <si>
+    <t>Heraklion, Greece</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/3rd-mediterranean-beach-games/results</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-45/results</t>
+  </si>
+  <si>
+    <t>Hangzhou, China</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/asian-games-0/results</t>
+  </si>
+  <si>
+    <t>U15, Veterans</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/world-championships-49/results</t>
+  </si>
+  <si>
+    <t>Veterans World Championships</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/veterans-world-championships/results</t>
+  </si>
+  <si>
+    <t>U23 World Championships</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/u23-world-championships/results</t>
+  </si>
+  <si>
+    <t>Arab Championship</t>
+  </si>
+  <si>
+    <t>Baghdad, Iraq</t>
+  </si>
+  <si>
+    <t>https://uww.org/event/arab-championship-10/results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -893,8 +1123,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1193,20 +1423,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1482,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1275,7 +1505,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1298,7 +1528,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1321,7 +1551,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1344,7 +1574,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1367,7 +1597,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1390,7 +1620,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1413,7 +1643,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1436,7 +1666,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1459,7 +1689,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1482,7 +1712,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1505,7 +1735,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1528,7 +1758,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1551,7 +1781,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1574,7 +1804,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1597,7 +1827,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1620,7 +1850,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1643,7 +1873,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1666,7 +1896,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1689,7 +1919,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1712,7 +1942,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1735,7 +1965,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -1758,7 +1988,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -1781,7 +2011,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1804,7 +2034,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -1827,7 +2057,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -1850,7 +2080,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -1873,7 +2103,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1896,7 +2126,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1919,7 +2149,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -1942,7 +2172,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -1965,7 +2195,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -1988,7 +2218,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -2011,7 +2241,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2034,7 +2264,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2057,7 +2287,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -2080,7 +2310,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>123</v>
       </c>
@@ -2103,7 +2333,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>126</v>
       </c>
@@ -2126,7 +2356,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2379,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>131</v>
       </c>
@@ -2172,7 +2402,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -2195,7 +2425,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -2218,7 +2448,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -2241,7 +2471,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -2264,7 +2494,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -2287,7 +2517,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -2310,7 +2540,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2333,7 +2563,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2356,7 +2586,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>149</v>
       </c>
@@ -2379,7 +2609,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -2402,7 +2632,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2425,7 +2655,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -2448,7 +2678,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -2464,14 +2694,14 @@
       <c r="E55" t="s">
         <v>25</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" t="s">
         <v>158</v>
       </c>
       <c r="G55">
         <v>2019</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -2494,7 +2724,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -2510,14 +2740,14 @@
       <c r="E57" t="s">
         <v>25</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" t="s">
         <v>162</v>
       </c>
       <c r="G57">
         <v>2019</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -2540,7 +2770,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -2563,7 +2793,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>168</v>
       </c>
@@ -2586,7 +2816,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>171</v>
       </c>
@@ -2609,7 +2839,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2632,7 +2862,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -2655,7 +2885,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>178</v>
       </c>
@@ -2678,7 +2908,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>21</v>
       </c>
@@ -2701,7 +2931,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -2724,7 +2954,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>35</v>
       </c>
@@ -2747,7 +2977,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>47</v>
       </c>
@@ -2770,7 +3000,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -2793,7 +3023,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -2816,7 +3046,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2839,7 +3069,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>192</v>
       </c>
@@ -2862,7 +3092,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>194</v>
       </c>
@@ -2885,7 +3115,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>196</v>
       </c>
@@ -2908,7 +3138,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2931,7 +3161,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -2954,7 +3184,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>201</v>
       </c>
@@ -2977,7 +3207,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -3000,7 +3230,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -3023,7 +3253,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>108</v>
       </c>
@@ -3046,7 +3276,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -3069,7 +3299,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>43</v>
       </c>
@@ -3092,7 +3322,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -3115,7 +3345,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -3138,7 +3368,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>213</v>
       </c>
@@ -3161,7 +3391,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -3184,7 +3414,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>120</v>
       </c>
@@ -3207,7 +3437,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>218</v>
       </c>
@@ -3230,7 +3460,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -3253,7 +3483,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -3276,7 +3506,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -3299,7 +3529,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>225</v>
       </c>
@@ -3322,7 +3552,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>228</v>
       </c>
@@ -3345,7 +3575,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>43</v>
       </c>
@@ -3368,7 +3598,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -3391,7 +3621,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>35</v>
       </c>
@@ -3414,7 +3644,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -3437,7 +3667,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>21</v>
       </c>
@@ -3460,7 +3690,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>238</v>
       </c>
@@ -3483,7 +3713,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -3506,7 +3736,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -3529,7 +3759,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>178</v>
       </c>
@@ -3552,7 +3782,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -3575,7 +3805,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>43</v>
       </c>
@@ -3598,7 +3828,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -3621,7 +3851,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -3644,7 +3874,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>250</v>
       </c>
@@ -3667,7 +3897,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>43</v>
       </c>
@@ -3690,7 +3920,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>85</v>
       </c>
@@ -3713,7 +3943,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>39</v>
       </c>
@@ -3736,7 +3966,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>85</v>
       </c>
@@ -3759,7 +3989,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>85</v>
       </c>
@@ -3782,7 +4012,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>85</v>
       </c>
@@ -3805,7 +4035,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>260</v>
       </c>
@@ -3828,7 +4058,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>85</v>
       </c>
@@ -3851,7 +4081,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>264</v>
       </c>
@@ -3874,25 +4104,920 @@
         <v>2022</v>
       </c>
     </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>267</v>
+      </c>
+      <c r="B117" t="s">
+        <v>86</v>
+      </c>
+      <c r="C117" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" t="s">
+        <v>25</v>
+      </c>
+      <c r="F117" t="s">
+        <v>268</v>
+      </c>
+      <c r="G117" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>270</v>
+      </c>
+      <c r="B118" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" t="s">
+        <v>25</v>
+      </c>
+      <c r="F118" t="s">
+        <v>272</v>
+      </c>
+      <c r="G118" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>43</v>
+      </c>
+      <c r="B119" t="s">
+        <v>132</v>
+      </c>
+      <c r="C119" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119" t="s">
+        <v>273</v>
+      </c>
+      <c r="F119" t="s">
+        <v>274</v>
+      </c>
+      <c r="G119" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>43</v>
+      </c>
+      <c r="B120" t="s">
+        <v>132</v>
+      </c>
+      <c r="C120" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" t="s">
+        <v>65</v>
+      </c>
+      <c r="E120" t="s">
+        <v>25</v>
+      </c>
+      <c r="F120" t="s">
+        <v>275</v>
+      </c>
+      <c r="G120" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121" t="s">
+        <v>276</v>
+      </c>
+      <c r="C121" t="s">
+        <v>23</v>
+      </c>
+      <c r="D121" t="s">
+        <v>10</v>
+      </c>
+      <c r="E121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F121" t="s">
+        <v>277</v>
+      </c>
+      <c r="G121" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>43</v>
+      </c>
+      <c r="B122" t="s">
+        <v>86</v>
+      </c>
+      <c r="C122" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" t="s">
+        <v>10</v>
+      </c>
+      <c r="E122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F122" t="s">
+        <v>278</v>
+      </c>
+      <c r="G122" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>279</v>
+      </c>
+      <c r="B123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>10</v>
+      </c>
+      <c r="E123" t="s">
+        <v>273</v>
+      </c>
+      <c r="F123" t="s">
+        <v>280</v>
+      </c>
+      <c r="G123" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>85</v>
+      </c>
+      <c r="B124" t="s">
+        <v>54</v>
+      </c>
+      <c r="C124" t="s">
+        <v>85</v>
+      </c>
+      <c r="D124" t="s">
+        <v>10</v>
+      </c>
+      <c r="E124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F124" t="s">
+        <v>282</v>
+      </c>
+      <c r="G124" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>47</v>
+      </c>
+      <c r="B125" t="s">
+        <v>127</v>
+      </c>
+      <c r="C125" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F125" t="s">
+        <v>283</v>
+      </c>
+      <c r="G125" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>21</v>
+      </c>
+      <c r="B126" t="s">
+        <v>145</v>
+      </c>
+      <c r="C126" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" t="s">
+        <v>180</v>
+      </c>
+      <c r="E126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F126" t="s">
+        <v>284</v>
+      </c>
+      <c r="G126" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>21</v>
+      </c>
+      <c r="B127" t="s">
+        <v>145</v>
+      </c>
+      <c r="C127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" t="s">
+        <v>10</v>
+      </c>
+      <c r="E127" t="s">
+        <v>285</v>
+      </c>
+      <c r="F127" t="s">
+        <v>286</v>
+      </c>
+      <c r="G127" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>287</v>
+      </c>
+      <c r="B128" t="s">
+        <v>36</v>
+      </c>
+      <c r="C128" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" t="s">
+        <v>25</v>
+      </c>
+      <c r="F128" t="s">
+        <v>288</v>
+      </c>
+      <c r="G128" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>35</v>
+      </c>
+      <c r="B129" t="s">
+        <v>36</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129" t="s">
+        <v>241</v>
+      </c>
+      <c r="E129" t="s">
+        <v>25</v>
+      </c>
+      <c r="F129" t="s">
+        <v>289</v>
+      </c>
+      <c r="G129" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>43</v>
+      </c>
+      <c r="B130" t="s">
+        <v>290</v>
+      </c>
+      <c r="C130" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130" t="s">
+        <v>52</v>
+      </c>
+      <c r="E130" t="s">
+        <v>25</v>
+      </c>
+      <c r="F130" t="s">
+        <v>291</v>
+      </c>
+      <c r="G130" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>35</v>
+      </c>
+      <c r="B131" t="s">
+        <v>276</v>
+      </c>
+      <c r="C131" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131" t="s">
+        <v>292</v>
+      </c>
+      <c r="E131" t="s">
+        <v>273</v>
+      </c>
+      <c r="F131" t="s">
+        <v>293</v>
+      </c>
+      <c r="G131" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>47</v>
+      </c>
+      <c r="B132" t="s">
+        <v>294</v>
+      </c>
+      <c r="C132" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" t="s">
+        <v>52</v>
+      </c>
+      <c r="E132" t="s">
+        <v>25</v>
+      </c>
+      <c r="F132" t="s">
+        <v>295</v>
+      </c>
+      <c r="G132" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>47</v>
+      </c>
+      <c r="B133" t="s">
+        <v>294</v>
+      </c>
+      <c r="C133" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133" t="s">
+        <v>52</v>
+      </c>
+      <c r="E133" t="s">
+        <v>285</v>
+      </c>
+      <c r="F133" t="s">
+        <v>296</v>
+      </c>
+      <c r="G133" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>43</v>
+      </c>
+      <c r="B134" t="s">
+        <v>297</v>
+      </c>
+      <c r="C134" t="s">
+        <v>23</v>
+      </c>
+      <c r="D134" t="s">
+        <v>92</v>
+      </c>
+      <c r="E134" t="s">
+        <v>25</v>
+      </c>
+      <c r="F134" t="s">
+        <v>298</v>
+      </c>
+      <c r="G134" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>299</v>
+      </c>
+      <c r="B135" t="s">
+        <v>145</v>
+      </c>
+      <c r="C135" t="s">
+        <v>41</v>
+      </c>
+      <c r="D135" t="s">
+        <v>10</v>
+      </c>
+      <c r="E135" t="s">
+        <v>285</v>
+      </c>
+      <c r="F135" t="s">
+        <v>300</v>
+      </c>
+      <c r="G135" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>43</v>
+      </c>
+      <c r="B136" t="s">
+        <v>301</v>
+      </c>
+      <c r="C136" t="s">
+        <v>45</v>
+      </c>
+      <c r="D136" t="s">
+        <v>302</v>
+      </c>
+      <c r="E136" t="s">
+        <v>285</v>
+      </c>
+      <c r="F136" t="s">
+        <v>303</v>
+      </c>
+      <c r="G136" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>304</v>
+      </c>
+      <c r="B137" t="s">
+        <v>301</v>
+      </c>
+      <c r="C137" t="s">
+        <v>305</v>
+      </c>
+      <c r="D137" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" t="s">
+        <v>285</v>
+      </c>
+      <c r="F137" t="s">
+        <v>306</v>
+      </c>
+      <c r="G137" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>307</v>
+      </c>
+      <c r="C138" t="s">
+        <v>23</v>
+      </c>
+      <c r="D138" t="s">
+        <v>92</v>
+      </c>
+      <c r="E138" t="s">
+        <v>25</v>
+      </c>
+      <c r="F138" t="s">
+        <v>308</v>
+      </c>
+      <c r="G138" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>43</v>
+      </c>
+      <c r="B139" t="s">
+        <v>309</v>
+      </c>
+      <c r="C139" t="s">
+        <v>23</v>
+      </c>
+      <c r="D139" t="s">
+        <v>74</v>
+      </c>
+      <c r="E139" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" t="s">
+        <v>310</v>
+      </c>
+      <c r="G139" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>35</v>
+      </c>
+      <c r="B140" t="s">
+        <v>311</v>
+      </c>
+      <c r="C140" t="s">
+        <v>23</v>
+      </c>
+      <c r="D140" t="s">
+        <v>247</v>
+      </c>
+      <c r="E140" t="s">
+        <v>25</v>
+      </c>
+      <c r="F140" t="s">
+        <v>312</v>
+      </c>
+      <c r="G140" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>313</v>
+      </c>
+      <c r="B141" t="s">
+        <v>129</v>
+      </c>
+      <c r="C141" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" t="s">
+        <v>25</v>
+      </c>
+      <c r="F141" t="s">
+        <v>314</v>
+      </c>
+      <c r="G141" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>315</v>
+      </c>
+      <c r="B142" t="s">
+        <v>316</v>
+      </c>
+      <c r="C142" t="s">
+        <v>41</v>
+      </c>
+      <c r="D142" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" t="s">
+        <v>317</v>
+      </c>
+      <c r="F142" t="s">
+        <v>318</v>
+      </c>
+      <c r="G142" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>85</v>
+      </c>
+      <c r="B143" t="s">
+        <v>64</v>
+      </c>
+      <c r="C143" t="s">
+        <v>85</v>
+      </c>
+      <c r="D143" t="s">
+        <v>52</v>
+      </c>
+      <c r="E143" t="s">
+        <v>25</v>
+      </c>
+      <c r="F143" t="s">
+        <v>319</v>
+      </c>
+      <c r="G143" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>58</v>
+      </c>
+      <c r="B144" t="s">
+        <v>320</v>
+      </c>
+      <c r="C144" t="s">
+        <v>23</v>
+      </c>
+      <c r="D144" t="s">
+        <v>180</v>
+      </c>
+      <c r="E144" t="s">
+        <v>25</v>
+      </c>
+      <c r="F144" t="s">
+        <v>321</v>
+      </c>
+      <c r="G144" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>85</v>
+      </c>
+      <c r="B145" t="s">
+        <v>311</v>
+      </c>
+      <c r="C145" t="s">
+        <v>85</v>
+      </c>
+      <c r="D145" t="s">
+        <v>92</v>
+      </c>
+      <c r="E145" t="s">
+        <v>25</v>
+      </c>
+      <c r="F145" t="s">
+        <v>322</v>
+      </c>
+      <c r="G145" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>85</v>
+      </c>
+      <c r="B146" t="s">
+        <v>109</v>
+      </c>
+      <c r="C146" t="s">
+        <v>85</v>
+      </c>
+      <c r="D146" t="s">
+        <v>180</v>
+      </c>
+      <c r="E146" t="s">
+        <v>273</v>
+      </c>
+      <c r="F146" t="s">
+        <v>323</v>
+      </c>
+      <c r="G146" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>324</v>
+      </c>
+      <c r="B147" t="s">
+        <v>325</v>
+      </c>
+      <c r="C147" t="s">
+        <v>41</v>
+      </c>
+      <c r="D147" t="s">
+        <v>10</v>
+      </c>
+      <c r="E147" t="s">
+        <v>19</v>
+      </c>
+      <c r="F147" t="s">
+        <v>326</v>
+      </c>
+      <c r="G147" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>85</v>
+      </c>
+      <c r="B148" t="s">
+        <v>327</v>
+      </c>
+      <c r="C148" t="s">
+        <v>45</v>
+      </c>
+      <c r="D148" t="s">
+        <v>302</v>
+      </c>
+      <c r="E148" t="s">
+        <v>285</v>
+      </c>
+      <c r="F148" t="s">
+        <v>328</v>
+      </c>
+      <c r="G148" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>329</v>
+      </c>
+      <c r="B149" t="s">
+        <v>330</v>
+      </c>
+      <c r="C149" t="s">
+        <v>41</v>
+      </c>
+      <c r="D149" t="s">
+        <v>10</v>
+      </c>
+      <c r="E149" t="s">
+        <v>285</v>
+      </c>
+      <c r="F149" t="s">
+        <v>331</v>
+      </c>
+      <c r="G149" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>85</v>
+      </c>
+      <c r="B150" t="s">
+        <v>189</v>
+      </c>
+      <c r="C150" t="s">
+        <v>85</v>
+      </c>
+      <c r="D150" t="s">
+        <v>10</v>
+      </c>
+      <c r="E150" t="s">
+        <v>25</v>
+      </c>
+      <c r="F150" t="s">
+        <v>332</v>
+      </c>
+      <c r="G150" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>105</v>
+      </c>
+      <c r="B151" t="s">
+        <v>333</v>
+      </c>
+      <c r="C151" t="s">
+        <v>41</v>
+      </c>
+      <c r="D151" t="s">
+        <v>10</v>
+      </c>
+      <c r="E151" t="s">
+        <v>25</v>
+      </c>
+      <c r="F151" t="s">
+        <v>334</v>
+      </c>
+      <c r="G151" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>85</v>
+      </c>
+      <c r="B152" t="s">
+        <v>222</v>
+      </c>
+      <c r="C152" t="s">
+        <v>85</v>
+      </c>
+      <c r="D152" t="s">
+        <v>335</v>
+      </c>
+      <c r="E152" t="s">
+        <v>273</v>
+      </c>
+      <c r="F152" t="s">
+        <v>336</v>
+      </c>
+      <c r="G152" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>337</v>
+      </c>
+      <c r="B153" t="s">
+        <v>222</v>
+      </c>
+      <c r="C153" t="s">
+        <v>85</v>
+      </c>
+      <c r="D153" t="s">
+        <v>118</v>
+      </c>
+      <c r="E153" t="s">
+        <v>83</v>
+      </c>
+      <c r="F153" t="s">
+        <v>338</v>
+      </c>
+      <c r="G153" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>339</v>
+      </c>
+      <c r="B154" t="s">
+        <v>290</v>
+      </c>
+      <c r="C154" t="s">
+        <v>85</v>
+      </c>
+      <c r="D154" t="s">
+        <v>65</v>
+      </c>
+      <c r="E154" t="s">
+        <v>25</v>
+      </c>
+      <c r="F154" t="s">
+        <v>340</v>
+      </c>
+      <c r="G154" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>341</v>
+      </c>
+      <c r="B155" t="s">
+        <v>342</v>
+      </c>
+      <c r="C155" t="s">
+        <v>9</v>
+      </c>
+      <c r="D155" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155" t="s">
+        <v>83</v>
+      </c>
+      <c r="F155" t="s">
+        <v>343</v>
+      </c>
+      <c r="G155" t="s">
+        <v>269</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{A82A4206-399B-4507-B716-C72E91C1C2F4}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{A1ED97B0-0B60-4F09-B1FF-9C9A4E18B04F}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{3C8F347D-CA9F-490C-8213-A81CB320AF61}"/>
-    <hyperlink ref="F35" r:id="rId4" xr:uid="{EF06FA33-6786-41D4-A6C2-DF10F263CAA4}"/>
-    <hyperlink ref="F34" r:id="rId5" xr:uid="{EEBCDC13-F747-4DE9-B9DD-178A46626C97}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{ADEFFBBB-6E71-41D5-BD70-23E692C719DA}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{1B1CDC27-2083-4CBB-87AE-15DBBC135AE4}"/>
-    <hyperlink ref="F31" r:id="rId8" xr:uid="{C7195C4A-FAEF-47FD-A294-63380420D5CC}"/>
-    <hyperlink ref="F32" r:id="rId9" xr:uid="{D2E36921-D5F8-4CFD-B2FC-F8F03372273A}"/>
-    <hyperlink ref="F46" r:id="rId10" xr:uid="{2696B7DC-056A-4D15-A00B-6A53CAE34FDC}"/>
-    <hyperlink ref="F47" r:id="rId11" xr:uid="{4BFF0159-9310-413D-8881-466F8768CAE0}"/>
-    <hyperlink ref="F48" r:id="rId12" xr:uid="{6E3E19C5-6FE1-484A-9F4E-C1DDF042866D}"/>
-    <hyperlink ref="F116" r:id="rId13" xr:uid="{7A29123E-4890-4BC8-8E20-194D42252243}"/>
-    <hyperlink ref="F61" r:id="rId14" xr:uid="{7B062950-F361-4611-9AB9-F4F8D590148A}"/>
-    <hyperlink ref="F56" r:id="rId15" xr:uid="{3F37A577-3985-4239-A4C1-86024AE46A51}"/>
-    <hyperlink ref="F55" r:id="rId16" xr:uid="{19F70462-35D8-4BB0-9F69-FB49124B0447}"/>
-    <hyperlink ref="F57" r:id="rId17" xr:uid="{4042D759-F035-46E4-BB65-DB5F38BAC02A}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F35" r:id="rId4"/>
+    <hyperlink ref="F34" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F31" r:id="rId8"/>
+    <hyperlink ref="F32" r:id="rId9"/>
+    <hyperlink ref="F46" r:id="rId10"/>
+    <hyperlink ref="F47" r:id="rId11"/>
+    <hyperlink ref="F48" r:id="rId12"/>
+    <hyperlink ref="F116" r:id="rId13"/>
+    <hyperlink ref="F61" r:id="rId14"/>
+    <hyperlink ref="F56" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>